<commit_message>
added platetype table creation and data load from excel
</commit_message>
<xml_diff>
--- a/src/main/resources/Utlity Table.xlsx
+++ b/src/main/resources/Utlity Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apolloits-my.sharepoint.com/personal/nischay_m_apolloits_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77883FE5-C0D8-45DB-8BCB-43D597F43182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41F2E54C-F225-4F40-9120-387EB950DA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-8340" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{68D5B328-6ABB-42A7-8ABA-2A0E36049037}"/>
+    <workbookView xWindow="22932" yWindow="-8340" windowWidth="30936" windowHeight="16776" firstSheet="1" activeTab="2" xr2:uid="{68D5B328-6ABB-42A7-8ABA-2A0E36049037}"/>
   </bookViews>
   <sheets>
     <sheet name="UtilityAgencyListing" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5282" uniqueCount="2441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5281" uniqueCount="2438">
   <si>
     <t>HomeAgency</t>
   </si>
@@ -557,12 +557,18 @@
     <t>ITAG_Valid</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>90</t>
   </si>
   <si>
     <t>ITAG_LOW_Bal</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
@@ -809,15 +815,9 @@
     <t>Specialty Plate (including organizational, motorcycles, trucks and other vehicle types)</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Passenger Standard and Vanity</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Temporary Plate</t>
   </si>
   <si>
@@ -7350,15 +7350,6 @@
   </si>
   <si>
     <t>Vietnam Veterans Of America Truck</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>[1]</t>
-  </si>
-  <si>
-    <t>NY could only have duplicates for plates that are 1-5 digits. Other plate numberings would not have duplicates and it would not be expected that alphanumeric plates or plates with 6 or more digits would have an associated LIC_TYPE in the ICLP file.</t>
   </si>
   <si>
     <t>LIC_TYPE</t>
@@ -7374,7 +7365,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7437,17 +7428,6 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -7512,7 +7492,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -7617,23 +7597,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -9824,8 +9792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F76E9A6-262D-46FC-96E3-D22B5FA83555}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9950,33 +9918,33 @@
       <c r="A11" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="19">
-        <v>1</v>
+      <c r="B11" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="19">
-        <v>2</v>
+        <v>172</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="19" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B13" s="19">
         <v>3</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -9986,659 +9954,659 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D70688-0E48-4467-94EF-9735DD34292D}">
-  <dimension ref="A1:E1220"/>
+  <dimension ref="A1:E1216"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A444" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C448" sqref="C448"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1217" sqref="A1217:XFD1222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.28515625" style="37" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" style="30" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="39" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="38" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="21" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D2" s="27"/>
       <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" ht="39">
       <c r="A3" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D22" s="27"/>
       <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D26" s="27"/>
       <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="28"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="28"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D32" s="27"/>
       <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D33" s="27"/>
       <c r="E33" s="28"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D34" s="27"/>
       <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D35" s="27"/>
       <c r="E35" s="28"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D36" s="27"/>
       <c r="E36" s="28"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D38" s="27"/>
       <c r="E38" s="28"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D39" s="27"/>
       <c r="E39" s="28"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D40" s="27"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D41" s="27"/>
       <c r="E41" s="28"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D42" s="27"/>
       <c r="E42" s="28"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D43" s="27"/>
       <c r="E43" s="28"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="28"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D45" s="27"/>
       <c r="E45" s="28"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D46" s="27"/>
       <c r="E46" s="28"/>
     </row>
     <row r="47" spans="1:5" ht="25.5">
       <c r="A47" s="25" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="25" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>254</v>
+        <v>170</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D48" s="27"/>
       <c r="E48" s="28"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="25" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>256</v>
+        <v>173</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>257</v>
@@ -10648,13 +10616,13 @@
     </row>
     <row r="50" spans="1:5" ht="39">
       <c r="A50" s="25" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D50" s="27" t="s">
         <v>258</v>
@@ -10692,10 +10660,10 @@
         <v>259</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D53" s="27" t="s">
         <v>264</v>
@@ -10811,7 +10779,7 @@
         <v>259</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C62" s="29" t="s">
         <v>281</v>
@@ -11024,7 +10992,7 @@
         <v>313</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="28"/>
@@ -11089,7 +11057,7 @@
         <v>322</v>
       </c>
       <c r="C83" s="29" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D83" s="27"/>
       <c r="E83" s="28"/>
@@ -11728,7 +11696,7 @@
         <v>420</v>
       </c>
       <c r="C132" s="27" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D132" s="27" t="s">
         <v>421</v>
@@ -12117,10 +12085,10 @@
         <v>471</v>
       </c>
       <c r="B162" s="26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C162" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D162" s="27"/>
       <c r="E162" s="28"/>
@@ -12133,7 +12101,7 @@
         <v>479</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D163" s="27"/>
       <c r="E163" s="28"/>
@@ -12250,7 +12218,7 @@
         <v>493</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D172" s="27"/>
       <c r="E172" s="28"/>
@@ -12276,7 +12244,7 @@
         <v>496</v>
       </c>
       <c r="C174" s="27" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D174" s="27"/>
       <c r="E174" s="28"/>
@@ -12289,7 +12257,7 @@
         <v>497</v>
       </c>
       <c r="C175" s="27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D175" s="27"/>
       <c r="E175" s="28"/>
@@ -12341,7 +12309,7 @@
         <v>504</v>
       </c>
       <c r="C179" s="27" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D179" s="27" t="s">
         <v>505</v>
@@ -12436,7 +12404,7 @@
         <v>518</v>
       </c>
       <c r="C186" s="27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D186" s="27"/>
       <c r="E186" s="28"/>
@@ -12598,7 +12566,7 @@
         <v>313</v>
       </c>
       <c r="C198" s="27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D198" s="27"/>
       <c r="E198" s="28"/>
@@ -12730,7 +12698,7 @@
         <v>552</v>
       </c>
       <c r="C208" s="27" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D208" s="27"/>
       <c r="E208" s="28"/>
@@ -12821,7 +12789,7 @@
         <v>561</v>
       </c>
       <c r="C215" s="27" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D215" s="27" t="s">
         <v>505</v>
@@ -12836,7 +12804,7 @@
         <v>562</v>
       </c>
       <c r="C216" s="27" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D216" s="27"/>
       <c r="E216" s="28"/>
@@ -12888,7 +12856,7 @@
         <v>569</v>
       </c>
       <c r="C220" s="27" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D220" s="27"/>
       <c r="E220" s="28"/>
@@ -12942,7 +12910,7 @@
         <v>360</v>
       </c>
       <c r="C224" s="27" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D224" s="27"/>
       <c r="E224" s="28"/>
@@ -13126,7 +13094,7 @@
         <v>599</v>
       </c>
       <c r="C238" s="27" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D238" s="27"/>
       <c r="E238" s="28"/>
@@ -13152,7 +13120,7 @@
         <v>601</v>
       </c>
       <c r="C240" s="27" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D240" s="27"/>
       <c r="E240" s="28"/>
@@ -13178,7 +13146,7 @@
         <v>604</v>
       </c>
       <c r="C242" s="27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D242" s="27"/>
       <c r="E242" s="28"/>
@@ -13243,7 +13211,7 @@
         <v>611</v>
       </c>
       <c r="C247" s="27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D247" s="27"/>
       <c r="E247" s="28"/>
@@ -13321,7 +13289,7 @@
         <v>622</v>
       </c>
       <c r="C253" s="27" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D253" s="27"/>
       <c r="E253" s="28"/>
@@ -13620,7 +13588,7 @@
         <v>665</v>
       </c>
       <c r="C276" s="27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D276" s="27"/>
       <c r="E276" s="28"/>
@@ -13763,7 +13731,7 @@
         <v>683</v>
       </c>
       <c r="C287" s="27" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D287" s="27"/>
       <c r="E287" s="28"/>
@@ -13854,7 +13822,7 @@
         <v>695</v>
       </c>
       <c r="C294" s="27" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D294" s="27"/>
       <c r="E294" s="28"/>
@@ -13867,7 +13835,7 @@
         <v>696</v>
       </c>
       <c r="C295" s="27" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D295" s="27"/>
       <c r="E295" s="28"/>
@@ -14036,7 +14004,7 @@
         <v>721</v>
       </c>
       <c r="C308" s="27" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D308" s="27"/>
       <c r="E308" s="28"/>
@@ -14049,7 +14017,7 @@
         <v>722</v>
       </c>
       <c r="C309" s="27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D309" s="27"/>
       <c r="E309" s="28"/>
@@ -14075,7 +14043,7 @@
         <v>725</v>
       </c>
       <c r="C311" s="27" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D311" s="27"/>
       <c r="E311" s="28"/>
@@ -14088,7 +14056,7 @@
         <v>726</v>
       </c>
       <c r="C312" s="27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D312" s="27"/>
       <c r="E312" s="28"/>
@@ -14179,7 +14147,7 @@
         <v>739</v>
       </c>
       <c r="C319" s="27" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D319" s="27"/>
       <c r="E319" s="28"/>
@@ -14348,7 +14316,7 @@
         <v>763</v>
       </c>
       <c r="C332" s="27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D332" s="27"/>
       <c r="E332" s="28"/>
@@ -14478,7 +14446,7 @@
         <v>782</v>
       </c>
       <c r="C342" s="27" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D342" s="27"/>
       <c r="E342" s="28"/>
@@ -14543,7 +14511,7 @@
         <v>791</v>
       </c>
       <c r="C347" s="27" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D347" s="27"/>
       <c r="E347" s="28"/>
@@ -14777,7 +14745,7 @@
         <v>824</v>
       </c>
       <c r="C365" s="27" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D365" s="27"/>
       <c r="E365" s="28"/>
@@ -14803,7 +14771,7 @@
         <v>826</v>
       </c>
       <c r="C367" s="27" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D367" s="27"/>
       <c r="E367" s="28"/>
@@ -14816,7 +14784,7 @@
         <v>827</v>
       </c>
       <c r="C368" s="27" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D368" s="27"/>
       <c r="E368" s="28"/>
@@ -14829,7 +14797,7 @@
         <v>828</v>
       </c>
       <c r="C369" s="27" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D369" s="27"/>
       <c r="E369" s="28"/>
@@ -14855,7 +14823,7 @@
         <v>831</v>
       </c>
       <c r="C371" s="27" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D371" s="27"/>
       <c r="E371" s="28"/>
@@ -14894,7 +14862,7 @@
         <v>837</v>
       </c>
       <c r="C374" s="27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D374" s="27"/>
       <c r="E374" s="28"/>
@@ -14907,7 +14875,7 @@
         <v>838</v>
       </c>
       <c r="C375" s="27" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D375" s="27"/>
       <c r="E375" s="28"/>
@@ -14920,7 +14888,7 @@
         <v>839</v>
       </c>
       <c r="C376" s="27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D376" s="27"/>
       <c r="E376" s="28"/>
@@ -14946,7 +14914,7 @@
         <v>842</v>
       </c>
       <c r="C378" s="27" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D378" s="27"/>
       <c r="E378" s="28"/>
@@ -14972,7 +14940,7 @@
         <v>845</v>
       </c>
       <c r="C380" s="27" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D380" s="27"/>
       <c r="E380" s="28"/>
@@ -15063,7 +15031,7 @@
         <v>858</v>
       </c>
       <c r="C387" s="27" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D387" s="27"/>
       <c r="E387" s="28"/>
@@ -15089,7 +15057,7 @@
         <v>861</v>
       </c>
       <c r="C389" s="27" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D389" s="27"/>
       <c r="E389" s="28"/>
@@ -15115,7 +15083,7 @@
         <v>864</v>
       </c>
       <c r="C391" s="27" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D391" s="27"/>
       <c r="E391" s="28"/>
@@ -15141,7 +15109,7 @@
         <v>867</v>
       </c>
       <c r="C393" s="27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D393" s="27"/>
       <c r="E393" s="28"/>
@@ -15154,7 +15122,7 @@
         <v>868</v>
       </c>
       <c r="C394" s="27" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D394" s="27"/>
       <c r="E394" s="28"/>
@@ -15206,7 +15174,7 @@
         <v>874</v>
       </c>
       <c r="C398" s="27" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D398" s="27"/>
       <c r="E398" s="28"/>
@@ -15349,7 +15317,7 @@
         <v>893</v>
       </c>
       <c r="C409" s="27" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D409" s="27"/>
       <c r="E409" s="28"/>
@@ -15375,7 +15343,7 @@
         <v>895</v>
       </c>
       <c r="C411" s="27" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D411" s="27"/>
       <c r="E411" s="28"/>
@@ -15388,7 +15356,7 @@
         <v>896</v>
       </c>
       <c r="C412" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D412" s="27"/>
       <c r="E412" s="28"/>
@@ -15760,7 +15728,7 @@
         <v>951</v>
       </c>
       <c r="C440" s="27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D440" s="27"/>
       <c r="E440" s="28"/>
@@ -19827,7 +19795,7 @@
         <v>313</v>
       </c>
       <c r="C749" s="27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D749" s="27"/>
       <c r="E749" s="28"/>
@@ -20707,7 +20675,7 @@
         <v>322</v>
       </c>
       <c r="C815" s="27" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D815" s="27"/>
       <c r="E815" s="28"/>
@@ -26279,30 +26247,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="1217" spans="1:5" s="30" customFormat="1">
-      <c r="A1217" s="37"/>
-      <c r="B1217" s="38"/>
-      <c r="E1217" s="39"/>
-    </row>
-    <row r="1219" spans="1:5">
-      <c r="A1219" s="40" t="s">
-        <v>2435</v>
-      </c>
-    </row>
-    <row r="1220" spans="1:5" ht="29.65" customHeight="1">
-      <c r="A1220" s="42" t="s">
-        <v>2436</v>
-      </c>
-      <c r="B1220" s="43" t="s">
-        <v>2437</v>
-      </c>
-      <c r="C1220" s="43"/>
-      <c r="D1220" s="43"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1220:D1220"/>
-  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
@@ -26324,232 +26269,232 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="16" t="s">
-        <v>2438</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" s="17" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" s="17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="17" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="17" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="17" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="17" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="17" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="17" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="17" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="17" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="17" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="17" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="17" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="17" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="17" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="17" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="17" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="17" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="17" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="17" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="17" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="17" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="17" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="17" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="17" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="17" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="17" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="17" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="17" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" s="17" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="17" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="17" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="17" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="17" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="17" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="17" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="2:2">
@@ -26569,7 +26514,7 @@
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="2:2">
@@ -26584,7 +26529,7 @@
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="2:2">
@@ -26629,7 +26574,7 @@
     </row>
     <row r="62" spans="2:2">
       <c r="B62" s="17" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="2:2">
@@ -27129,7 +27074,7 @@
     </row>
     <row r="162" spans="2:2">
       <c r="B162" s="17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="163" spans="2:2">
@@ -32422,7 +32367,7 @@
   <sheetData>
     <row r="1" spans="2:2" ht="48.75" customHeight="1">
       <c r="B1" s="15" t="s">
-        <v>2439</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="2" spans="2:2">
@@ -33132,7 +33077,7 @@
   <sheetData>
     <row r="3" spans="3:3">
       <c r="C3" t="s">
-        <v>2440</v>
+        <v>2437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed observation IAGA-082,83,84,85,86 and 77
</commit_message>
<xml_diff>
--- a/src/main/resources/Utlity Table.xlsx
+++ b/src/main/resources/Utlity Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28521"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apolloits-my.sharepoint.com/personal/nischay_m_apolloits_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50CB2BA6-6DA1-4D10-9AEA-8932829B75FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F4A7BEF-A12B-4FCB-872F-1163D13DFE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-8340" windowWidth="30936" windowHeight="16776" firstSheet="2" activeTab="2" xr2:uid="{68D5B328-6ABB-42A7-8ABA-2A0E36049037}"/>
+    <workbookView xWindow="22932" yWindow="-8340" windowWidth="30936" windowHeight="16776" xr2:uid="{68D5B328-6ABB-42A7-8ABA-2A0E36049037}"/>
   </bookViews>
   <sheets>
     <sheet name="UtilityAgencyListing" sheetId="1" r:id="rId1"/>
@@ -393,10 +393,10 @@
     <t>SRTA</t>
   </si>
   <si>
-    <t>0010110001</t>
-  </si>
-  <si>
-    <t>0099990002</t>
+    <t>0000110001</t>
+  </si>
+  <si>
+    <t>0009990002</t>
   </si>
   <si>
     <t>0035</t>
@@ -8102,8 +8102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB6E20C-A33D-40AF-8C7C-658D7F955B95}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9897,8 +9897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F76E9A6-262D-46FC-96E3-D22B5FA83555}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10061,7 +10061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D70688-0E48-4467-94EF-9735DD34292D}">
   <dimension ref="A1:E1277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1277" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A1217" sqref="A1217:A1277"/>
     </sheetView>

</xml_diff>